<commit_message>
ajuste do botao de inserir romaneio
</commit_message>
<xml_diff>
--- a/Massa de Dados Profectum.xlsx
+++ b/Massa de Dados Profectum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbara\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03CAD571-5CAD-4139-BCDB-BF2333CF7187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED9EE8C-501D-4060-9581-6B0A5CC4771B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3BE345D7-41E4-4CA8-8FD6-9D27C9C2A3A1}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="20760" windowHeight="11070" xr2:uid="{3BE345D7-41E4-4CA8-8FD6-9D27C9C2A3A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
   <si>
-    <t>Identificador</t>
-  </si>
-  <si>
     <t>Tipo do Movtº</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>000283386</t>
+  </si>
+  <si>
+    <t>Nota</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -669,617 +669,617 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>9590659</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4">
         <v>45839</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>9593201</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4">
         <v>45840</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>9593752</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4">
         <v>45840</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>9593871</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>45840</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>9594728</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4">
         <v>45841</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9595677</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4">
         <v>45841</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>9595718</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4">
         <v>45841</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="G8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>9623790</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4">
         <v>45854</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9628237</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4">
         <v>45855</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9685947</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="4">
         <v>45860</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9698907</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="4">
         <v>45887</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>9658635</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4">
         <v>45869</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>9723605</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>9693920</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="4">
         <v>45884</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>9707199</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4">
         <v>45890</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>9715382</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="4">
         <v>45894</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="G17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>9718499</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4">
         <v>45895</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>9621523</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="4">
         <v>45853</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>9627636</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="4">
         <v>45855</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G20" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>9628531</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="4">
         <v>45855</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>9629986</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="4">
         <v>45856</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G22" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>9654472</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="4">
         <v>45868</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>